<commit_message>
Ejecutar el script de Preprocesamiento y Limpieza de Datos
</commit_message>
<xml_diff>
--- a/src/static/xlsx/cleaned_data.xlsx
+++ b/src/static/xlsx/cleaned_data.xlsx
@@ -572,7 +572,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.137765</t>
+          <t>2025-03-15T21:10:27.346654</t>
         </is>
       </c>
       <c r="O2" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.145201</t>
+          <t>2025-03-15T21:10:27.346654</t>
         </is>
       </c>
       <c r="O3" t="n">
@@ -710,7 +710,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.153499</t>
+          <t>2025-03-15T21:10:27.346654</t>
         </is>
       </c>
       <c r="O4" t="n">
@@ -779,7 +779,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.159540</t>
+          <t>2025-03-15T21:10:27.346654</t>
         </is>
       </c>
       <c r="O5" t="n">
@@ -848,7 +848,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.165728</t>
+          <t>2025-03-15T21:10:27.346654</t>
         </is>
       </c>
       <c r="O6" t="n">
@@ -917,7 +917,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.173087</t>
+          <t>2025-03-15T21:10:27.346654</t>
         </is>
       </c>
       <c r="O7" t="n">
@@ -986,7 +986,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.178660</t>
+          <t>2025-03-15T21:10:27.346654</t>
         </is>
       </c>
       <c r="O8" t="n">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.184775</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O9" t="n">
@@ -1124,7 +1124,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.189975</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O10" t="n">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.197908</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O11" t="n">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.203854</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O12" t="n">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.208251</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O13" t="n">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.214443</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O14" t="n">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.220600</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O15" t="n">
@@ -1509,7 +1509,7 @@
         <v>555988</v>
       </c>
       <c r="H16" t="n">
-        <v>4052.652145857761</v>
+        <v>4033</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1538,11 +1538,11 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.227278</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O16" t="n">
-        <v>137.1911479173653</v>
+        <v>137.8596578229606</v>
       </c>
     </row>
     <row r="17">
@@ -1607,7 +1607,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.231968</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O17" t="n">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.237754</t>
+          <t>2025-03-15T21:10:27.362280</t>
         </is>
       </c>
       <c r="O18" t="n">
@@ -1713,7 +1713,7 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>25987</v>
+        <v>26096</v>
       </c>
       <c r="H19" t="n">
         <v>328</v>
@@ -1745,11 +1745,11 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.244852</t>
+          <t>2025-03-15T21:10:27.377900</t>
         </is>
       </c>
       <c r="O19" t="n">
-        <v>79.22865853658537</v>
+        <v>79.5609756097561</v>
       </c>
     </row>
     <row r="20">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.252355</t>
+          <t>2025-03-15T21:10:27.377900</t>
         </is>
       </c>
       <c r="O20" t="n">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.257762</t>
+          <t>2025-03-15T21:10:27.377900</t>
         </is>
       </c>
       <c r="O21" t="n">
@@ -1952,7 +1952,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.263673</t>
+          <t>2025-03-15T21:10:27.377900</t>
         </is>
       </c>
       <c r="O22" t="n">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.268387</t>
+          <t>2025-03-15T21:10:27.377900</t>
         </is>
       </c>
       <c r="O23" t="n">
@@ -2090,7 +2090,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.274430</t>
+          <t>2025-03-15T21:10:27.377900</t>
         </is>
       </c>
       <c r="O24" t="n">
@@ -2159,7 +2159,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.279657</t>
+          <t>2025-03-15T21:10:27.377900</t>
         </is>
       </c>
       <c r="O25" t="n">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.285035</t>
+          <t>2025-03-15T21:10:27.377900</t>
         </is>
       </c>
       <c r="O26" t="n">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.291934</t>
+          <t>2025-03-15T21:10:27.393528</t>
         </is>
       </c>
       <c r="O27" t="n">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.297294</t>
+          <t>2025-03-15T21:10:27.393528</t>
         </is>
       </c>
       <c r="O28" t="n">
@@ -2415,7 +2415,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>["Skopje"]</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.303333</t>
+          <t>2025-03-15T21:10:27.393528</t>
         </is>
       </c>
       <c r="O29" t="n">
@@ -2504,7 +2504,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.307813</t>
+          <t>2025-03-15T21:10:27.393528</t>
         </is>
       </c>
       <c r="O30" t="n">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.314496</t>
+          <t>2025-03-15T21:10:27.393528</t>
         </is>
       </c>
       <c r="O31" t="n">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.321479</t>
+          <t>2025-03-15T21:10:27.393528</t>
         </is>
       </c>
       <c r="O32" t="n">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.328029</t>
+          <t>2025-03-15T21:10:27.393528</t>
         </is>
       </c>
       <c r="O33" t="n">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.332693</t>
+          <t>2025-03-15T21:10:27.393528</t>
         </is>
       </c>
       <c r="O34" t="n">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.339545</t>
+          <t>2025-03-15T21:10:27.393528</t>
         </is>
       </c>
       <c r="O35" t="n">
@@ -2918,7 +2918,7 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.344855</t>
+          <t>2025-03-15T21:10:27.409158</t>
         </is>
       </c>
       <c r="O36" t="n">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.350575</t>
+          <t>2025-03-15T21:10:27.409158</t>
         </is>
       </c>
       <c r="O37" t="n">
@@ -3024,7 +3024,7 @@
         </is>
       </c>
       <c r="G38" t="n">
-        <v>102334403</v>
+        <v>103940191</v>
       </c>
       <c r="H38" t="n">
         <v>1002450</v>
@@ -3056,11 +3056,11 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.357699</t>
+          <t>2025-03-15T21:10:27.409158</t>
         </is>
       </c>
       <c r="O38" t="n">
-        <v>102.0842964736396</v>
+        <v>103.6861599082249</v>
       </c>
     </row>
     <row r="39">
@@ -3125,7 +3125,7 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.364484</t>
+          <t>2025-03-15T21:10:27.409158</t>
         </is>
       </c>
       <c r="O39" t="n">
@@ -3194,7 +3194,7 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.370485</t>
+          <t>2025-03-15T21:10:27.409158</t>
         </is>
       </c>
       <c r="O40" t="n">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.376909</t>
+          <t>2025-03-15T21:10:27.409158</t>
         </is>
       </c>
       <c r="O41" t="n">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.386025</t>
+          <t>2025-03-15T21:10:27.409158</t>
         </is>
       </c>
       <c r="O42" t="n">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.391739</t>
+          <t>2025-03-15T21:10:27.409158</t>
         </is>
       </c>
       <c r="O43" t="n">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>["Singapore"]</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3470,7 +3470,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.398080</t>
+          <t>2025-03-15T21:10:27.424783</t>
         </is>
       </c>
       <c r="O44" t="n">
@@ -3539,7 +3539,7 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.405884</t>
+          <t>2025-03-15T21:10:27.424783</t>
         </is>
       </c>
       <c r="O45" t="n">
@@ -3608,7 +3608,7 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.410433</t>
+          <t>2025-03-15T21:10:27.424783</t>
         </is>
       </c>
       <c r="O46" t="n">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.417125</t>
+          <t>2025-03-15T21:10:27.424783</t>
         </is>
       </c>
       <c r="O47" t="n">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.422807</t>
+          <t>2025-03-15T21:10:27.424783</t>
         </is>
       </c>
       <c r="O48" t="n">
@@ -3795,7 +3795,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>["London"]</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -3815,7 +3815,7 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.427629</t>
+          <t>2025-03-15T21:10:27.424783</t>
         </is>
       </c>
       <c r="O49" t="n">
@@ -3884,7 +3884,7 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.433130</t>
+          <t>2025-03-15T21:10:27.424783</t>
         </is>
       </c>
       <c r="O50" t="n">
@@ -3953,7 +3953,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.438284</t>
+          <t>2025-03-15T21:10:27.424783</t>
         </is>
       </c>
       <c r="O51" t="n">
@@ -4022,7 +4022,7 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.444509</t>
+          <t>2025-03-15T21:10:27.424783</t>
         </is>
       </c>
       <c r="O52" t="n">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.451677</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O53" t="n">
@@ -4160,7 +4160,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.458069</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O54" t="n">
@@ -4229,7 +4229,7 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.466081</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O55" t="n">
@@ -4298,7 +4298,7 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.471837</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O56" t="n">
@@ -4367,7 +4367,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.477574</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O57" t="n">
@@ -4436,7 +4436,7 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.483862</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O58" t="n">
@@ -4505,7 +4505,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.488232</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O59" t="n">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.497774</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O60" t="n">
@@ -4643,7 +4643,7 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.504836</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O61" t="n">
@@ -4712,7 +4712,7 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.512548</t>
+          <t>2025-03-15T21:10:27.440398</t>
         </is>
       </c>
       <c r="O62" t="n">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.519637</t>
+          <t>2025-03-15T21:10:27.456029</t>
         </is>
       </c>
       <c r="O63" t="n">
@@ -4850,7 +4850,7 @@
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.525769</t>
+          <t>2025-03-15T21:10:27.456029</t>
         </is>
       </c>
       <c r="O64" t="n">
@@ -4919,7 +4919,7 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.533311</t>
+          <t>2025-03-15T21:10:27.456029</t>
         </is>
       </c>
       <c r="O65" t="n">
@@ -4959,7 +4959,7 @@
         <v>36910558</v>
       </c>
       <c r="H66" t="n">
-        <v>446550</v>
+        <v>456230.4782380175</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
@@ -4988,11 +4988,11 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.541424</t>
+          <t>2025-03-15T21:10:27.456029</t>
         </is>
       </c>
       <c r="O66" t="n">
-        <v>82.65716717052962</v>
+        <v>80.90331479507951</v>
       </c>
     </row>
     <row r="67">
@@ -5057,7 +5057,7 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.547681</t>
+          <t>2025-03-15T21:10:27.456029</t>
         </is>
       </c>
       <c r="O67" t="n">
@@ -5126,7 +5126,7 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.553019</t>
+          <t>2025-03-15T21:10:27.456029</t>
         </is>
       </c>
       <c r="O68" t="n">
@@ -5195,7 +5195,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.559899</t>
+          <t>2025-03-15T21:10:27.456029</t>
         </is>
       </c>
       <c r="O69" t="n">
@@ -5264,7 +5264,7 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.565448</t>
+          <t>2025-03-15T21:10:27.456029</t>
         </is>
       </c>
       <c r="O70" t="n">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.571951</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O71" t="n">
@@ -5402,7 +5402,7 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.578752</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O72" t="n">
@@ -5471,7 +5471,7 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.586986</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O73" t="n">
@@ -5540,7 +5540,7 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.594690</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O74" t="n">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.601820</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O75" t="n">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.609758</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O76" t="n">
@@ -5747,7 +5747,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.617483</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O77" t="n">
@@ -5816,7 +5816,7 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.623322</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O78" t="n">
@@ -5885,7 +5885,7 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.631238</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O79" t="n">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.641796</t>
+          <t>2025-03-15T21:10:27.471647</t>
         </is>
       </c>
       <c r="O80" t="n">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.648742</t>
+          <t>2025-03-15T21:10:27.487284</t>
         </is>
       </c>
       <c r="O81" t="n">
@@ -6092,7 +6092,7 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.655039</t>
+          <t>2025-03-15T21:10:27.487284</t>
         </is>
       </c>
       <c r="O82" t="n">
@@ -6161,7 +6161,7 @@
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.660066</t>
+          <t>2025-03-15T21:10:27.487284</t>
         </is>
       </c>
       <c r="O83" t="n">
@@ -6230,7 +6230,7 @@
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.667946</t>
+          <t>2025-03-15T21:10:27.487284</t>
         </is>
       </c>
       <c r="O84" t="n">
@@ -6299,7 +6299,7 @@
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.674670</t>
+          <t>2025-03-15T21:10:27.487284</t>
         </is>
       </c>
       <c r="O85" t="n">
@@ -6368,7 +6368,7 @@
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.682794</t>
+          <t>2025-03-15T21:10:27.487284</t>
         </is>
       </c>
       <c r="O86" t="n">
@@ -6437,7 +6437,7 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.689559</t>
+          <t>2025-03-15T21:10:27.487284</t>
         </is>
       </c>
       <c r="O87" t="n">
@@ -6506,7 +6506,7 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.696034</t>
+          <t>2025-03-15T21:10:27.502908</t>
         </is>
       </c>
       <c r="O88" t="n">
@@ -6575,7 +6575,7 @@
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.701893</t>
+          <t>2025-03-15T21:10:27.502908</t>
         </is>
       </c>
       <c r="O89" t="n">
@@ -6644,7 +6644,7 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.707923</t>
+          <t>2025-03-15T21:10:27.502908</t>
         </is>
       </c>
       <c r="O90" t="n">
@@ -6713,7 +6713,7 @@
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.723983</t>
+          <t>2025-03-15T21:10:27.502908</t>
         </is>
       </c>
       <c r="O91" t="n">
@@ -6782,7 +6782,7 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.732929</t>
+          <t>2025-03-15T21:10:27.502908</t>
         </is>
       </c>
       <c r="O92" t="n">
@@ -6851,7 +6851,7 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.739863</t>
+          <t>2025-03-15T21:10:27.502908</t>
         </is>
       </c>
       <c r="O93" t="n">
@@ -6920,7 +6920,7 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.746356</t>
+          <t>2025-03-15T21:10:27.502908</t>
         </is>
       </c>
       <c r="O94" t="n">
@@ -6989,7 +6989,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.753050</t>
+          <t>2025-03-15T21:10:27.502908</t>
         </is>
       </c>
       <c r="O95" t="n">
@@ -7058,7 +7058,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.760724</t>
+          <t>2025-03-15T21:10:27.502908</t>
         </is>
       </c>
       <c r="O96" t="n">
@@ -7127,7 +7127,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.767034</t>
+          <t>2025-03-15T21:10:27.518525</t>
         </is>
       </c>
       <c r="O97" t="n">
@@ -7196,7 +7196,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.774877</t>
+          <t>2025-03-15T21:10:27.518525</t>
         </is>
       </c>
       <c r="O98" t="n">
@@ -7265,7 +7265,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.782536</t>
+          <t>2025-03-15T21:10:27.518525</t>
         </is>
       </c>
       <c r="O99" t="n">
@@ -7334,7 +7334,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.787850</t>
+          <t>2025-03-15T21:10:27.518525</t>
         </is>
       </c>
       <c r="O100" t="n">
@@ -7403,7 +7403,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.794641</t>
+          <t>2025-03-15T21:10:27.518525</t>
         </is>
       </c>
       <c r="O101" t="n">
@@ -7472,7 +7472,7 @@
       </c>
       <c r="N102" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.801481</t>
+          <t>2025-03-15T21:10:27.518525</t>
         </is>
       </c>
       <c r="O102" t="n">
@@ -7541,7 +7541,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.808757</t>
+          <t>2025-03-15T21:10:27.518525</t>
         </is>
       </c>
       <c r="O103" t="n">
@@ -7610,7 +7610,7 @@
       </c>
       <c r="N104" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.814768</t>
+          <t>2025-03-15T21:10:27.518525</t>
         </is>
       </c>
       <c r="O104" t="n">
@@ -7679,7 +7679,7 @@
       </c>
       <c r="N105" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.822860</t>
+          <t>2025-03-15T21:10:27.518525</t>
         </is>
       </c>
       <c r="O105" t="n">
@@ -7748,7 +7748,7 @@
       </c>
       <c r="N106" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.833231</t>
+          <t>2025-03-15T21:10:27.534148</t>
         </is>
       </c>
       <c r="O106" t="n">
@@ -7817,7 +7817,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.841436</t>
+          <t>2025-03-15T21:10:27.534148</t>
         </is>
       </c>
       <c r="O107" t="n">
@@ -7886,7 +7886,7 @@
       </c>
       <c r="N108" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.847953</t>
+          <t>2025-03-15T21:10:27.534148</t>
         </is>
       </c>
       <c r="O108" t="n">
@@ -7955,7 +7955,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.854598</t>
+          <t>2025-03-15T21:10:27.534148</t>
         </is>
       </c>
       <c r="O109" t="n">
@@ -8024,7 +8024,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.861439</t>
+          <t>2025-03-15T21:10:27.534148</t>
         </is>
       </c>
       <c r="O110" t="n">
@@ -8093,7 +8093,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.869774</t>
+          <t>2025-03-15T21:10:27.534148</t>
         </is>
       </c>
       <c r="O111" t="n">
@@ -8162,7 +8162,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.876723</t>
+          <t>2025-03-15T21:10:27.534148</t>
         </is>
       </c>
       <c r="O112" t="n">
@@ -8231,7 +8231,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.882299</t>
+          <t>2025-03-15T21:10:27.534148</t>
         </is>
       </c>
       <c r="O113" t="n">
@@ -8300,7 +8300,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.887985</t>
+          <t>2025-03-15T21:10:27.534148</t>
         </is>
       </c>
       <c r="O114" t="n">
@@ -8369,7 +8369,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.892540</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O115" t="n">
@@ -8438,7 +8438,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.897973</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O116" t="n">
@@ -8507,7 +8507,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.903650</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O117" t="n">
@@ -8540,7 +8540,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>North America</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="G118" t="n">
@@ -8576,7 +8576,7 @@
       </c>
       <c r="N118" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.909484</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O118" t="n">
@@ -8645,7 +8645,7 @@
       </c>
       <c r="N119" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.916310</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O119" t="n">
@@ -8714,7 +8714,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.921846</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O120" t="n">
@@ -8783,7 +8783,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.927156</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O121" t="n">
@@ -8852,7 +8852,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.932717</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O122" t="n">
@@ -8921,7 +8921,7 @@
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.938013</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O123" t="n">
@@ -8990,7 +8990,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.944178</t>
+          <t>2025-03-15T21:10:27.549773</t>
         </is>
       </c>
       <c r="O124" t="n">
@@ -9059,7 +9059,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.949784</t>
+          <t>2025-03-15T21:10:27.565402</t>
         </is>
       </c>
       <c r="O125" t="n">
@@ -9128,7 +9128,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.956562</t>
+          <t>2025-03-15T21:10:27.565402</t>
         </is>
       </c>
       <c r="O126" t="n">
@@ -9197,7 +9197,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.963010</t>
+          <t>2025-03-15T21:10:27.565402</t>
         </is>
       </c>
       <c r="O127" t="n">
@@ -9266,7 +9266,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.969448</t>
+          <t>2025-03-15T21:10:27.565402</t>
         </is>
       </c>
       <c r="O128" t="n">
@@ -9335,7 +9335,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.975785</t>
+          <t>2025-03-15T21:10:27.565402</t>
         </is>
       </c>
       <c r="O129" t="n">
@@ -9404,7 +9404,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.981448</t>
+          <t>2025-03-15T21:10:27.565402</t>
         </is>
       </c>
       <c r="O130" t="n">
@@ -9473,7 +9473,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.985813</t>
+          <t>2025-03-15T21:10:27.565402</t>
         </is>
       </c>
       <c r="O131" t="n">
@@ -9542,7 +9542,7 @@
       </c>
       <c r="N132" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.991786</t>
+          <t>2025-03-15T21:10:27.565402</t>
         </is>
       </c>
       <c r="O132" t="n">
@@ -9575,7 +9575,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Australia and New Zealand</t>
         </is>
       </c>
       <c r="G133" t="n">
@@ -9611,7 +9611,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:18.997102</t>
+          <t>2025-03-15T21:10:27.565402</t>
         </is>
       </c>
       <c r="O133" t="n">
@@ -9680,7 +9680,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.004756</t>
+          <t>2025-03-15T21:10:27.581027</t>
         </is>
       </c>
       <c r="O134" t="n">
@@ -9749,7 +9749,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.011054</t>
+          <t>2025-03-15T21:10:27.581027</t>
         </is>
       </c>
       <c r="O135" t="n">
@@ -9786,7 +9786,7 @@
         </is>
       </c>
       <c r="G136" t="n">
-        <v>11523</v>
+        <v>11792</v>
       </c>
       <c r="H136" t="n">
         <v>26</v>
@@ -9818,11 +9818,11 @@
       </c>
       <c r="N136" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.016427</t>
+          <t>2025-03-15T21:10:27.581027</t>
         </is>
       </c>
       <c r="O136" t="n">
-        <v>443.1923076923077</v>
+        <v>453.5384615384615</v>
       </c>
     </row>
     <row r="137">
@@ -9887,7 +9887,7 @@
       </c>
       <c r="N137" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.022877</t>
+          <t>2025-03-15T21:10:27.581027</t>
         </is>
       </c>
       <c r="O137" t="n">
@@ -9956,7 +9956,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.030881</t>
+          <t>2025-03-15T21:10:27.581027</t>
         </is>
       </c>
       <c r="O138" t="n">
@@ -10025,7 +10025,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.036828</t>
+          <t>2025-03-15T21:10:27.581027</t>
         </is>
       </c>
       <c r="O139" t="n">
@@ -10094,7 +10094,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.041728</t>
+          <t>2025-03-15T21:10:27.581027</t>
         </is>
       </c>
       <c r="O140" t="n">
@@ -10163,7 +10163,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.046932</t>
+          <t>2025-03-15T21:10:27.581027</t>
         </is>
       </c>
       <c r="O141" t="n">
@@ -10232,7 +10232,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.056011</t>
+          <t>2025-03-15T21:10:27.581027</t>
         </is>
       </c>
       <c r="O142" t="n">
@@ -10301,7 +10301,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.061401</t>
+          <t>2025-03-15T21:10:27.596651</t>
         </is>
       </c>
       <c r="O143" t="n">
@@ -10370,7 +10370,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.066658</t>
+          <t>2025-03-15T21:10:27.596651</t>
         </is>
       </c>
       <c r="O144" t="n">
@@ -10439,7 +10439,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.071764</t>
+          <t>2025-03-15T21:10:27.596651</t>
         </is>
       </c>
       <c r="O145" t="n">
@@ -10508,7 +10508,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.077273</t>
+          <t>2025-03-15T21:10:27.596651</t>
         </is>
       </c>
       <c r="O146" t="n">
@@ -10577,7 +10577,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.083455</t>
+          <t>2025-03-15T21:10:27.596651</t>
         </is>
       </c>
       <c r="O147" t="n">
@@ -10646,7 +10646,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.088064</t>
+          <t>2025-03-15T21:10:27.596651</t>
         </is>
       </c>
       <c r="O148" t="n">
@@ -10686,7 +10686,7 @@
         <v>13132792</v>
       </c>
       <c r="H149" t="n">
-        <v>239380.8728852471</v>
+        <v>245857</v>
       </c>
       <c r="I149" t="inlineStr">
         <is>
@@ -10715,11 +10715,11 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.092836</t>
+          <t>2025-03-15T21:10:27.596651</t>
         </is>
       </c>
       <c r="O149" t="n">
-        <v>54.86149265691548</v>
+        <v>53.41638432096707</v>
       </c>
     </row>
     <row r="150">
@@ -10784,7 +10784,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.101437</t>
+          <t>2025-03-15T21:10:27.596651</t>
         </is>
       </c>
       <c r="O150" t="n">
@@ -10853,7 +10853,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.107175</t>
+          <t>2025-03-15T21:10:27.612277</t>
         </is>
       </c>
       <c r="O151" t="n">
@@ -10922,7 +10922,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.111957</t>
+          <t>2025-03-15T21:10:27.612277</t>
         </is>
       </c>
       <c r="O152" t="n">
@@ -10991,7 +10991,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.117255</t>
+          <t>2025-03-15T21:10:27.612277</t>
         </is>
       </c>
       <c r="O153" t="n">
@@ -11060,7 +11060,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.123168</t>
+          <t>2025-03-15T21:10:27.612277</t>
         </is>
       </c>
       <c r="O154" t="n">
@@ -11129,7 +11129,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.129710</t>
+          <t>2025-03-15T21:10:27.612277</t>
         </is>
       </c>
       <c r="O155" t="n">
@@ -11198,7 +11198,7 @@
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.135445</t>
+          <t>2025-03-15T21:10:27.612277</t>
         </is>
       </c>
       <c r="O156" t="n">
@@ -11267,7 +11267,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.142557</t>
+          <t>2025-03-15T21:10:27.612277</t>
         </is>
       </c>
       <c r="O157" t="n">
@@ -11300,11 +11300,11 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>Western Africa</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="G158" t="n">
-        <v>8095686</v>
+        <v>8278737</v>
       </c>
       <c r="H158" t="n">
         <v>56785</v>
@@ -11336,11 +11336,11 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.149580</t>
+          <t>2025-03-15T21:10:27.612277</t>
         </is>
       </c>
       <c r="O158" t="n">
-        <v>142.5673329224267</v>
+        <v>145.7909130932464</v>
       </c>
     </row>
     <row r="159">
@@ -11405,7 +11405,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.155181</t>
+          <t>2025-03-15T21:10:27.612277</t>
         </is>
       </c>
       <c r="O159" t="n">
@@ -11474,7 +11474,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.162534</t>
+          <t>2025-03-15T21:10:27.627910</t>
         </is>
       </c>
       <c r="O160" t="n">
@@ -11543,7 +11543,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.168083</t>
+          <t>2025-03-15T21:10:27.627910</t>
         </is>
       </c>
       <c r="O161" t="n">
@@ -11612,7 +11612,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.174524</t>
+          <t>2025-03-15T21:10:27.627910</t>
         </is>
       </c>
       <c r="O162" t="n">
@@ -11681,7 +11681,7 @@
       </c>
       <c r="N163" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.180404</t>
+          <t>2025-03-15T21:10:27.627910</t>
         </is>
       </c>
       <c r="O163" t="n">
@@ -11750,7 +11750,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.187057</t>
+          <t>2025-03-15T21:10:27.627910</t>
         </is>
       </c>
       <c r="O164" t="n">
@@ -11799,7 +11799,7 @@
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>["Bucharest"]</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
@@ -11819,7 +11819,7 @@
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.193309</t>
+          <t>2025-03-15T21:10:27.627910</t>
         </is>
       </c>
       <c r="O165" t="n">
@@ -11888,7 +11888,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.199491</t>
+          <t>2025-03-15T21:10:27.627910</t>
         </is>
       </c>
       <c r="O166" t="n">
@@ -11957,7 +11957,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.205498</t>
+          <t>2025-03-15T21:10:27.627910</t>
         </is>
       </c>
       <c r="O167" t="n">
@@ -11990,7 +11990,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>South-Eastern Asia</t>
         </is>
       </c>
       <c r="G168" t="n">
@@ -12026,7 +12026,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.210718</t>
+          <t>2025-03-15T21:10:27.627910</t>
         </is>
       </c>
       <c r="O168" t="n">
@@ -12095,7 +12095,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.216498</t>
+          <t>2025-03-15T21:10:27.643529</t>
         </is>
       </c>
       <c r="O169" t="n">
@@ -12164,7 +12164,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.222067</t>
+          <t>2025-03-15T21:10:27.643529</t>
         </is>
       </c>
       <c r="O170" t="n">
@@ -12233,7 +12233,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.226654</t>
+          <t>2025-03-15T21:10:27.643529</t>
         </is>
       </c>
       <c r="O171" t="n">
@@ -12302,7 +12302,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.232710</t>
+          <t>2025-03-15T21:10:27.643529</t>
         </is>
       </c>
       <c r="O172" t="n">
@@ -12371,7 +12371,7 @@
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.241252</t>
+          <t>2025-03-15T21:10:27.643529</t>
         </is>
       </c>
       <c r="O173" t="n">
@@ -12440,7 +12440,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.250622</t>
+          <t>2025-03-15T21:10:27.643529</t>
         </is>
       </c>
       <c r="O174" t="n">
@@ -12509,7 +12509,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.256847</t>
+          <t>2025-03-15T21:10:27.643529</t>
         </is>
       </c>
       <c r="O175" t="n">
@@ -12549,7 +12549,7 @@
         <v>31255435</v>
       </c>
       <c r="H176" t="n">
-        <v>801590</v>
+        <v>807435.5331000228</v>
       </c>
       <c r="I176" t="inlineStr">
         <is>
@@ -12578,11 +12578,11 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.262907</t>
+          <t>2025-03-15T21:10:27.643529</t>
         </is>
       </c>
       <c r="O176" t="n">
-        <v>38.99179755236467</v>
+        <v>38.70951143306715</v>
       </c>
     </row>
     <row r="177">
@@ -12647,7 +12647,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.269523</t>
+          <t>2025-03-15T21:10:27.643529</t>
         </is>
       </c>
       <c r="O177" t="n">
@@ -12716,7 +12716,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.276326</t>
+          <t>2025-03-15T21:10:27.659155</t>
         </is>
       </c>
       <c r="O178" t="n">
@@ -12785,7 +12785,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.283768</t>
+          <t>2025-03-15T21:10:27.659155</t>
         </is>
       </c>
       <c r="O179" t="n">
@@ -12854,7 +12854,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.291657</t>
+          <t>2025-03-15T21:10:27.659155</t>
         </is>
       </c>
       <c r="O180" t="n">
@@ -12923,7 +12923,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.297457</t>
+          <t>2025-03-15T21:10:27.659155</t>
         </is>
       </c>
       <c r="O181" t="n">
@@ -12992,7 +12992,7 @@
       </c>
       <c r="N182" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.303251</t>
+          <t>2025-03-15T21:10:27.659155</t>
         </is>
       </c>
       <c r="O182" t="n">
@@ -13061,7 +13061,7 @@
       </c>
       <c r="N183" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.310760</t>
+          <t>2025-03-15T21:10:27.659155</t>
         </is>
       </c>
       <c r="O183" t="n">
@@ -13130,7 +13130,7 @@
       </c>
       <c r="N184" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.318511</t>
+          <t>2025-03-15T21:10:27.659155</t>
         </is>
       </c>
       <c r="O184" t="n">
@@ -13199,7 +13199,7 @@
       </c>
       <c r="N185" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.325872</t>
+          <t>2025-03-15T21:10:27.659155</t>
         </is>
       </c>
       <c r="O185" t="n">
@@ -13268,7 +13268,7 @@
       </c>
       <c r="N186" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.333687</t>
+          <t>2025-03-15T21:10:27.659155</t>
         </is>
       </c>
       <c r="O186" t="n">
@@ -13337,7 +13337,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.339750</t>
+          <t>2025-03-15T21:10:27.674776</t>
         </is>
       </c>
       <c r="O187" t="n">
@@ -13406,7 +13406,7 @@
       </c>
       <c r="N188" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.346829</t>
+          <t>2025-03-15T21:10:27.674776</t>
         </is>
       </c>
       <c r="O188" t="n">
@@ -13475,7 +13475,7 @@
       </c>
       <c r="N189" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.353447</t>
+          <t>2025-03-15T21:10:27.674776</t>
         </is>
       </c>
       <c r="O189" t="n">
@@ -13544,7 +13544,7 @@
       </c>
       <c r="N190" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.360451</t>
+          <t>2025-03-15T21:10:27.674776</t>
         </is>
       </c>
       <c r="O190" t="n">
@@ -13613,7 +13613,7 @@
       </c>
       <c r="N191" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.367744</t>
+          <t>2025-03-15T21:10:27.674776</t>
         </is>
       </c>
       <c r="O191" t="n">
@@ -13682,7 +13682,7 @@
       </c>
       <c r="N192" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.373949</t>
+          <t>2025-03-15T21:10:27.674776</t>
         </is>
       </c>
       <c r="O192" t="n">
@@ -13751,7 +13751,7 @@
       </c>
       <c r="N193" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.382475</t>
+          <t>2025-03-15T21:10:27.674776</t>
         </is>
       </c>
       <c r="O193" t="n">
@@ -13820,7 +13820,7 @@
       </c>
       <c r="N194" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.388381</t>
+          <t>2025-03-15T21:10:27.674776</t>
         </is>
       </c>
       <c r="O194" t="n">
@@ -13889,7 +13889,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.394593</t>
+          <t>2025-03-15T21:10:27.674776</t>
         </is>
       </c>
       <c r="O195" t="n">
@@ -13958,7 +13958,7 @@
       </c>
       <c r="N196" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.401791</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O196" t="n">
@@ -14027,7 +14027,7 @@
       </c>
       <c r="N197" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.407770</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O197" t="n">
@@ -14096,7 +14096,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.414234</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O198" t="n">
@@ -14165,7 +14165,7 @@
       </c>
       <c r="N199" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.422740</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O199" t="n">
@@ -14234,7 +14234,7 @@
       </c>
       <c r="N200" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.433398</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O200" t="n">
@@ -14303,7 +14303,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.440562</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O201" t="n">
@@ -14372,7 +14372,7 @@
       </c>
       <c r="N202" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.446027</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O202" t="n">
@@ -14441,7 +14441,7 @@
       </c>
       <c r="N203" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.452382</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O203" t="n">
@@ -14510,7 +14510,7 @@
       </c>
       <c r="N204" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.458354</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O204" t="n">
@@ -14579,7 +14579,7 @@
       </c>
       <c r="N205" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.463983</t>
+          <t>2025-03-15T21:10:27.690407</t>
         </is>
       </c>
       <c r="O205" t="n">
@@ -14648,7 +14648,7 @@
       </c>
       <c r="N206" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.472436</t>
+          <t>2025-03-15T21:10:27.706029</t>
         </is>
       </c>
       <c r="O206" t="n">
@@ -14717,7 +14717,7 @@
       </c>
       <c r="N207" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.477176</t>
+          <t>2025-03-15T21:10:27.706029</t>
         </is>
       </c>
       <c r="O207" t="n">
@@ -14786,7 +14786,7 @@
       </c>
       <c r="N208" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.482944</t>
+          <t>2025-03-15T21:10:27.706029</t>
         </is>
       </c>
       <c r="O208" t="n">
@@ -14855,7 +14855,7 @@
       </c>
       <c r="N209" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.488044</t>
+          <t>2025-03-15T21:10:27.706029</t>
         </is>
       </c>
       <c r="O209" t="n">
@@ -14924,7 +14924,7 @@
       </c>
       <c r="N210" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.494881</t>
+          <t>2025-03-15T21:10:27.706029</t>
         </is>
       </c>
       <c r="O210" t="n">
@@ -14993,7 +14993,7 @@
       </c>
       <c r="N211" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.502080</t>
+          <t>2025-03-15T21:10:27.706029</t>
         </is>
       </c>
       <c r="O211" t="n">
@@ -15062,7 +15062,7 @@
       </c>
       <c r="N212" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.509355</t>
+          <t>2025-03-15T21:10:27.706029</t>
         </is>
       </c>
       <c r="O212" t="n">
@@ -15131,7 +15131,7 @@
       </c>
       <c r="N213" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.518605</t>
+          <t>2025-03-15T21:10:27.706029</t>
         </is>
       </c>
       <c r="O213" t="n">
@@ -15200,7 +15200,7 @@
       </c>
       <c r="N214" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.524496</t>
+          <t>2025-03-15T21:10:27.706029</t>
         </is>
       </c>
       <c r="O214" t="n">
@@ -15269,7 +15269,7 @@
       </c>
       <c r="N215" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.531734</t>
+          <t>2025-03-15T21:10:27.721650</t>
         </is>
       </c>
       <c r="O215" t="n">
@@ -15338,7 +15338,7 @@
       </c>
       <c r="N216" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.537838</t>
+          <t>2025-03-15T21:10:27.721650</t>
         </is>
       </c>
       <c r="O216" t="n">
@@ -15407,7 +15407,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.544429</t>
+          <t>2025-03-15T21:10:27.721650</t>
         </is>
       </c>
       <c r="O217" t="n">
@@ -15476,7 +15476,7 @@
       </c>
       <c r="N218" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.550045</t>
+          <t>2025-03-15T21:10:27.721650</t>
         </is>
       </c>
       <c r="O218" t="n">
@@ -15545,7 +15545,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.556279</t>
+          <t>2025-03-15T21:10:27.721650</t>
         </is>
       </c>
       <c r="O219" t="n">
@@ -15614,7 +15614,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.564402</t>
+          <t>2025-03-15T21:10:27.721650</t>
         </is>
       </c>
       <c r="O220" t="n">
@@ -15683,7 +15683,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.570789</t>
+          <t>2025-03-15T21:10:27.721650</t>
         </is>
       </c>
       <c r="O221" t="n">
@@ -15752,7 +15752,7 @@
       </c>
       <c r="N222" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.576246</t>
+          <t>2025-03-15T21:10:27.721650</t>
         </is>
       </c>
       <c r="O222" t="n">
@@ -15821,7 +15821,7 @@
       </c>
       <c r="N223" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.581428</t>
+          <t>2025-03-15T21:10:27.721650</t>
         </is>
       </c>
       <c r="O223" t="n">
@@ -15890,7 +15890,7 @@
       </c>
       <c r="N224" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.587867</t>
+          <t>2025-03-15T21:10:27.737276</t>
         </is>
       </c>
       <c r="O224" t="n">
@@ -15959,7 +15959,7 @@
       </c>
       <c r="N225" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.593854</t>
+          <t>2025-03-15T21:10:27.737276</t>
         </is>
       </c>
       <c r="O225" t="n">
@@ -16028,7 +16028,7 @@
       </c>
       <c r="N226" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.599915</t>
+          <t>2025-03-15T21:10:27.737276</t>
         </is>
       </c>
       <c r="O226" t="n">
@@ -16097,7 +16097,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.606340</t>
+          <t>2025-03-15T21:10:27.737276</t>
         </is>
       </c>
       <c r="O227" t="n">
@@ -16166,7 +16166,7 @@
       </c>
       <c r="N228" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.612537</t>
+          <t>2025-03-15T21:10:27.737276</t>
         </is>
       </c>
       <c r="O228" t="n">
@@ -16235,7 +16235,7 @@
       </c>
       <c r="N229" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.617797</t>
+          <t>2025-03-15T21:10:27.737276</t>
         </is>
       </c>
       <c r="O229" t="n">
@@ -16304,7 +16304,7 @@
       </c>
       <c r="N230" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.624494</t>
+          <t>2025-03-15T21:10:27.737276</t>
         </is>
       </c>
       <c r="O230" t="n">
@@ -16373,7 +16373,7 @@
       </c>
       <c r="N231" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.630635</t>
+          <t>2025-03-15T21:10:27.737276</t>
         </is>
       </c>
       <c r="O231" t="n">
@@ -16442,7 +16442,7 @@
       </c>
       <c r="N232" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.636409</t>
+          <t>2025-03-15T21:10:27.752944</t>
         </is>
       </c>
       <c r="O232" t="n">
@@ -16511,7 +16511,7 @@
       </c>
       <c r="N233" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.641778</t>
+          <t>2025-03-15T21:10:27.752944</t>
         </is>
       </c>
       <c r="O233" t="n">
@@ -16580,7 +16580,7 @@
       </c>
       <c r="N234" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.647908</t>
+          <t>2025-03-15T21:10:27.752944</t>
         </is>
       </c>
       <c r="O234" t="n">
@@ -16649,7 +16649,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.653847</t>
+          <t>2025-03-15T21:10:27.752944</t>
         </is>
       </c>
       <c r="O235" t="n">
@@ -16718,7 +16718,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.662279</t>
+          <t>2025-03-15T21:10:27.752944</t>
         </is>
       </c>
       <c r="O236" t="n">
@@ -16787,7 +16787,7 @@
       </c>
       <c r="N237" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.673401</t>
+          <t>2025-03-15T21:10:27.752944</t>
         </is>
       </c>
       <c r="O237" t="n">
@@ -16856,7 +16856,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.679565</t>
+          <t>2025-03-15T21:10:27.752944</t>
         </is>
       </c>
       <c r="O238" t="n">
@@ -16925,7 +16925,7 @@
       </c>
       <c r="N239" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.685932</t>
+          <t>2025-03-15T21:10:27.752944</t>
         </is>
       </c>
       <c r="O239" t="n">
@@ -16994,7 +16994,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.691633</t>
+          <t>2025-03-15T21:10:27.752944</t>
         </is>
       </c>
       <c r="O240" t="n">
@@ -17063,7 +17063,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.697000</t>
+          <t>2025-03-15T21:10:27.768617</t>
         </is>
       </c>
       <c r="O241" t="n">
@@ -17132,7 +17132,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.704674</t>
+          <t>2025-03-15T21:10:27.770451</t>
         </is>
       </c>
       <c r="O242" t="n">
@@ -17201,7 +17201,7 @@
       </c>
       <c r="N243" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.710557</t>
+          <t>2025-03-15T21:10:27.770451</t>
         </is>
       </c>
       <c r="O243" t="n">
@@ -17270,7 +17270,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.716063</t>
+          <t>2025-03-15T21:10:27.770451</t>
         </is>
       </c>
       <c r="O244" t="n">
@@ -17339,7 +17339,7 @@
       </c>
       <c r="N245" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.721776</t>
+          <t>2025-03-15T21:10:27.770451</t>
         </is>
       </c>
       <c r="O245" t="n">
@@ -17408,7 +17408,7 @@
       </c>
       <c r="N246" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.728120</t>
+          <t>2025-03-15T21:10:27.770451</t>
         </is>
       </c>
       <c r="O246" t="n">
@@ -17477,7 +17477,7 @@
       </c>
       <c r="N247" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.735275</t>
+          <t>2025-03-15T21:10:27.770451</t>
         </is>
       </c>
       <c r="O247" t="n">
@@ -17546,7 +17546,7 @@
       </c>
       <c r="N248" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.741560</t>
+          <t>2025-03-15T21:10:27.770451</t>
         </is>
       </c>
       <c r="O248" t="n">
@@ -17615,7 +17615,7 @@
       </c>
       <c r="N249" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.752599</t>
+          <t>2025-03-15T21:10:27.770451</t>
         </is>
       </c>
       <c r="O249" t="n">
@@ -17684,7 +17684,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.758780</t>
+          <t>2025-03-15T21:10:27.770451</t>
         </is>
       </c>
       <c r="O250" t="n">
@@ -17753,7 +17753,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>2025-03-15T15:59:19.764733</t>
+          <t>2025-03-15T21:10:27.786130</t>
         </is>
       </c>
       <c r="O251" t="n">

</xml_diff>